<commit_message>
diageous, fix things and copy to integ
</commit_message>
<xml_diff>
--- a/Projects/INTEG41/Data/on_premise Template.xlsx
+++ b/Projects/INTEG41/Data/on_premise Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>KPI Name</t>
   </si>
@@ -49,13 +49,16 @@
     <t>POD</t>
   </si>
   <si>
+    <t>Store Score</t>
+  </si>
+  <si>
+    <t>1. Back Bar</t>
+  </si>
+  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>Back Bar</t>
-  </si>
-  <si>
-    <t>1. Back Bar</t>
   </si>
   <si>
     <t>Menu</t>
@@ -282,15 +285,15 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.5263157894737"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="76.8056680161943"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
@@ -347,12 +350,16 @@
         <v>8</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H4" s="5" t="n">
         <v>0.5</v>
@@ -360,38 +367,42 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="D6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>9</v>
+      <c r="G6" s="5" t="n">
+        <v>0.25</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>